<commit_message>
non room non fonctionnelle
</commit_message>
<xml_diff>
--- a/messages.xlsx
+++ b/messages.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Documents\GitHub\interactive-box\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="7590" windowHeight="3270"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>Emitter</t>
   </si>
@@ -117,9 +122,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,14 +160,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -201,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,43 +466,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -486,7 +511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -497,7 +522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -505,7 +530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -513,7 +538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -524,193 +549,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -718,6 +586,9 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
       <c r="G20" t="s">
         <v>28</v>
       </c>
@@ -725,9 +596,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -742,30 +613,204 @@
         <v>29</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refonte sessions et modif good/bad réponse
</commit_message>
<xml_diff>
--- a/messages.xlsx
+++ b/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
   <si>
     <t>Emitter</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>File R</t>
+  </si>
+  <si>
+    <t>arrayOfGoodAnswers</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -690,6 +693,9 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -703,6 +709,9 @@
       </c>
       <c r="D19" t="s">
         <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
L'écran utilisateur annonce si on a une bonne ou une mauvaise réponse
Signed-off-by: antoineb19 <antoinebenoit@msn.com>
</commit_message>
<xml_diff>
--- a/messages.xlsx
+++ b/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
   <si>
     <t>Emitter</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Commentaires</t>
-  </si>
-  <si>
     <t>confirmConnection</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>all-users-are-ready</t>
   </si>
   <si>
-    <t>réponses</t>
-  </si>
-  <si>
     <t>answer</t>
   </si>
   <si>
@@ -115,6 +109,15 @@
   </si>
   <si>
     <t>arrayOfGoodAnswers</t>
+  </si>
+  <si>
+    <t>réponses, time</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
+  <si>
+    <t>end-time-request</t>
   </si>
 </sst>
 </file>
@@ -150,8 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,19 +450,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -472,283 +478,320 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>